<commit_message>
Add missing 7x7x7 for Geoff Hartnell
</commit_message>
<xml_diff>
--- a/data/2021-09-04/SCW Weekly Comp 2021-09-06 (Responses).xlsx
+++ b/data/2021-09-04/SCW Weekly Comp 2021-09-06 (Responses).xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$DF$71</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$DF$72</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="248">
   <si>
     <t>Timestamp</t>
   </si>
@@ -742,6 +742,21 @@
   </si>
   <si>
     <t>https://www.facebook.com/events/208105634636421/?post_id=216790703767914&amp;view=permalink&amp;__cft__[0]=AZXmrDZ88uTvHox3B7412poeuqK5qjb3y8ugnhIUzgmPsQ5ws46hUdHFdy-eJvq6TdiYoO7Z0cijDYnda2QGBJPB6_h4eHALixylPvcGPwdVqyh_mscSwEluRSjuFDIAGIU&amp;__tn__=%2CO%2CP-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/899313470960376/permalink/900960417462348/</t>
+  </si>
+  <si>
+    <t>5:37.78</t>
+  </si>
+  <si>
+    <t>4:53.38</t>
+  </si>
+  <si>
+    <t>4:51.45</t>
+  </si>
+  <si>
+    <t>5:07.54</t>
   </si>
 </sst>
 </file>
@@ -4111,8 +4126,43 @@
         <v>31.91</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" s="2">
+        <v>44462.49572644676</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="AO72" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="AP72" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="AQ72" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="AR72" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="AS72" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$DF$71"/>
+  <autoFilter ref="$A$1:$DF$72"/>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F2"/>
     <hyperlink r:id="rId2" ref="F3"/>
@@ -4184,7 +4234,8 @@
     <hyperlink r:id="rId68" ref="F69"/>
     <hyperlink r:id="rId69" ref="F70"/>
     <hyperlink r:id="rId70" ref="F71"/>
+    <hyperlink r:id="rId71" ref="F72"/>
   </hyperlinks>
-  <drawing r:id="rId71"/>
+  <drawing r:id="rId72"/>
 </worksheet>
 </file>
</xml_diff>